<commit_message>
add red valve and burner usage
</commit_message>
<xml_diff>
--- a/anaconda-projects/dashboard-cv-furnace/Burners_settings_vs_O2 _rev1.xlsx
+++ b/anaconda-projects/dashboard-cv-furnace/Burners_settings_vs_O2 _rev1.xlsx
@@ -20,211 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Temperature </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">setpoint / degC</t>
-    </r>
+    <t xml:space="preserve">Temperature setpoint / degC</t>
   </si>
   <si>
     <t xml:space="preserve">Burners in use</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Burner </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">approx value</t>
-    </r>
+    <t xml:space="preserve">Burner approx value</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Burner t</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">urns from zero</t>
-    </r>
+    <t xml:space="preserve">Burner turns from zero</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Fan s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">etpoint / %</t>
-    </r>
+    <t xml:space="preserve">Red valve</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Fan </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">speed / RPM</t>
-    </r>
+    <t xml:space="preserve">Fan setpoint / %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan speed / RPM</t>
   </si>
   <si>
     <t xml:space="preserve">Pressure setpoint / Pa</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">damper range / % (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">low)</t>
-    </r>
+    <t xml:space="preserve"> damper range / % (low)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">damper range / % (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">High)</t>
-    </r>
+    <t xml:space="preserve">damper range / % (High)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Output </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">O2 / %</t>
-    </r>
+    <t xml:space="preserve">Output O2 / %</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Output </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Burner usage / %</t>
-    </r>
+    <t xml:space="preserve">Output Burner usage / %</t>
   </si>
 </sst>
 </file>
@@ -235,7 +66,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -257,12 +88,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -382,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,7 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -415,11 +240,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,11 +248,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,15 +260,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,26 +357,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R14" activeCellId="0" sqref="R14"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.56640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="12.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="13.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="14.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="11.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="14.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="13.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="14.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,32 +387,35 @@
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,28 +431,31 @@
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="F2" s="13" t="n">
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="G2" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G2" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H2" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I2" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J2" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="J2" s="5" t="n">
+      <c r="K2" s="5" t="n">
         <v>4.1</v>
       </c>
-      <c r="K2" s="5" t="n">
+      <c r="L2" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -646,28 +470,31 @@
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="15" t="n">
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13" t="n">
         <v>65</v>
       </c>
-      <c r="F3" s="15" t="n">
+      <c r="G3" s="13" t="n">
         <v>1914</v>
       </c>
-      <c r="G3" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H3" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I3" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J3" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="J3" s="5" t="n">
+      <c r="K3" s="5" t="n">
         <v>3.6</v>
       </c>
-      <c r="K3" s="5" t="n">
+      <c r="L3" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="L3" s="14"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -676,34 +503,37 @@
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="n">
+      <c r="C4" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="n">
+      <c r="D4" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="G4" s="3" t="n">
         <v>1914</v>
       </c>
-      <c r="G4" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H4" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J4" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="K4" s="5" t="n">
         <v>3.4</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="L4" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="L4" s="14"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -712,34 +542,37 @@
       <c r="B5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="n">
+      <c r="C5" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="16" t="n">
+      <c r="D5" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="G5" s="3" t="n">
         <v>1914</v>
       </c>
-      <c r="G5" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H5" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J5" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="K5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="L5" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="L5" s="14"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -754,28 +587,31 @@
       <c r="D6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="15" t="n">
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13" t="n">
         <v>50</v>
       </c>
-      <c r="F6" s="15" t="n">
+      <c r="G6" s="13" t="n">
         <v>1473</v>
       </c>
-      <c r="G6" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H6" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I6" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J6" s="4" t="n">
         <v>95</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="K6" s="5" t="n">
         <v>1.85</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="L6" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="L6" s="14"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -790,28 +626,31 @@
       <c r="D7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="G7" s="3" t="n">
         <v>1473</v>
       </c>
-      <c r="G7" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H7" s="4" t="n">
-        <v>80</v>
-      </c>
-      <c r="I7" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="J7" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>80</v>
+      </c>
+      <c r="J7" s="15" t="n">
+        <v>96</v>
+      </c>
+      <c r="K7" s="5" t="n">
         <v>1.9</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="L7" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -820,34 +659,37 @@
       <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="14" t="n">
         <v>4.5</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="G8" s="3" t="n">
         <v>1473</v>
       </c>
-      <c r="G8" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H8" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J8" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K8" s="5" t="n">
         <v>1.45</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="L8" s="5" t="n">
         <v>40.5</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -856,34 +698,37 @@
       <c r="B9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="16" t="n">
+      <c r="C9" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="G9" s="3" t="n">
         <v>1473</v>
       </c>
-      <c r="G9" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H9" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J9" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K9" s="5" t="n">
         <v>1.15</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="L9" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -892,34 +737,37 @@
       <c r="B10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="18" t="n">
+      <c r="C10" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="D10" s="18" t="n">
+      <c r="D10" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="E10" s="15" t="n">
+      <c r="E10" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13" t="n">
         <v>45</v>
       </c>
-      <c r="F10" s="15" t="n">
+      <c r="G10" s="13" t="n">
         <v>1325</v>
       </c>
-      <c r="G10" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H10" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J10" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K10" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="L10" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="L10" s="14"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -928,34 +776,37 @@
       <c r="B11" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="18" t="n">
+      <c r="C11" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="D11" s="18" t="n">
+      <c r="D11" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="E11" s="15" t="n">
+      <c r="E11" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13" t="n">
         <v>47</v>
       </c>
-      <c r="F11" s="15" t="n">
+      <c r="G11" s="13" t="n">
         <v>1384</v>
       </c>
-      <c r="G11" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H11" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J11" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K11" s="5" t="n">
         <v>0.6</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="L11" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="L11" s="14"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -964,34 +815,37 @@
       <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="16" t="n">
+      <c r="C12" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="E12" s="15" t="n">
+      <c r="E12" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13" t="n">
         <v>50</v>
       </c>
-      <c r="F12" s="15" t="n">
+      <c r="G12" s="13" t="n">
         <v>1473</v>
       </c>
-      <c r="G12" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H12" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J12" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J12" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K12" s="5" t="n">
         <v>1.8</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="L12" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="L12" s="14"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -1000,34 +854,37 @@
       <c r="B13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="18" t="n">
+      <c r="C13" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="18" t="n">
+      <c r="D13" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="15" t="n">
+      <c r="E13" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13" t="n">
         <v>53</v>
       </c>
-      <c r="F13" s="15" t="n">
+      <c r="G13" s="13" t="n">
         <v>1561</v>
       </c>
-      <c r="G13" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H13" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J13" s="5" t="n">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>96</v>
       </c>
       <c r="K13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="5" t="n">
         <v>43</v>
       </c>
-      <c r="L13" s="14"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1036,34 +893,37 @@
       <c r="B14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15" t="n">
-        <v>80</v>
-      </c>
-      <c r="F14" s="15" t="n">
+      <c r="C14" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13" t="n">
+        <v>80</v>
+      </c>
+      <c r="G14" s="13" t="n">
         <v>2356</v>
       </c>
-      <c r="G14" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H14" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J14" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K14" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="L14" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1072,34 +932,37 @@
       <c r="B15" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="16" t="n">
+      <c r="C15" s="14" t="n">
         <v>-1</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="14" t="n">
         <v>-2</v>
       </c>
-      <c r="E15" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F15" s="13" t="n">
+      <c r="E15" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G15" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G15" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H15" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J15" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J15" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K15" s="5" t="n">
         <v>4.15</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="L15" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="L15" s="14"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1108,34 +971,37 @@
       <c r="B16" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="16" t="n">
+      <c r="C16" s="14" t="n">
         <v>-3</v>
       </c>
-      <c r="D16" s="16" t="n">
+      <c r="D16" s="14" t="n">
         <v>-5</v>
       </c>
-      <c r="E16" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F16" s="13" t="n">
+      <c r="E16" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G16" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G16" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H16" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J16" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J16" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K16" s="5" t="n">
         <v>4.5</v>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="L16" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="L16" s="14"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1144,34 +1010,37 @@
       <c r="B17" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="16" t="n">
+      <c r="C17" s="14" t="n">
         <v>-6</v>
       </c>
-      <c r="D17" s="16" t="n">
+      <c r="D17" s="14" t="n">
         <v>-9</v>
       </c>
-      <c r="E17" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F17" s="13" t="n">
+      <c r="E17" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G17" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G17" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H17" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J17" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J17" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K17" s="5" t="n">
         <v>5.1</v>
       </c>
-      <c r="K17" s="5" t="n">
+      <c r="L17" s="5" t="n">
         <v>41</v>
       </c>
-      <c r="L17" s="14"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1180,34 +1049,37 @@
       <c r="B18" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="18" t="n">
+      <c r="C18" s="16" t="n">
         <v>-6</v>
       </c>
-      <c r="D18" s="18" t="n">
+      <c r="D18" s="16" t="n">
         <v>-9</v>
       </c>
-      <c r="E18" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F18" s="13" t="n">
+      <c r="E18" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G18" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G18" s="4" t="n">
-        <v>20</v>
-      </c>
       <c r="H18" s="4" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>96</v>
-      </c>
-      <c r="J18" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J18" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="K18" s="5" t="n">
         <v>9.1</v>
       </c>
-      <c r="K18" s="5" t="n">
+      <c r="L18" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="L18" s="14"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1216,34 +1088,37 @@
       <c r="B19" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C19" s="16" t="n">
+      <c r="C19" s="14" t="n">
         <v>-3</v>
       </c>
-      <c r="D19" s="16" t="n">
+      <c r="D19" s="14" t="n">
         <v>-5</v>
       </c>
-      <c r="E19" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F19" s="13" t="n">
+      <c r="E19" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G19" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G19" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H19" s="17" t="n">
+      <c r="H19" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I19" s="15" t="n">
         <v>50</v>
       </c>
-      <c r="I19" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="15" t="n">
+        <v>96</v>
+      </c>
+      <c r="K19" s="5" t="n">
         <v>8.7</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="L19" s="5" t="n">
         <v>89</v>
       </c>
-      <c r="L19" s="14"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1252,34 +1127,37 @@
       <c r="B20" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C20" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="13" t="n">
-        <v>80</v>
-      </c>
-      <c r="F20" s="13" t="n">
+      <c r="C20" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11" t="n">
+        <v>80</v>
+      </c>
+      <c r="G20" s="11" t="n">
         <v>2356</v>
       </c>
-      <c r="G20" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H20" s="19" t="n">
+      <c r="H20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I20" s="17" t="n">
         <v>50</v>
       </c>
-      <c r="I20" s="19" t="n">
-        <v>96</v>
-      </c>
-      <c r="J20" s="5" t="n">
+      <c r="J20" s="17" t="n">
+        <v>96</v>
+      </c>
+      <c r="K20" s="5" t="n">
         <v>8.1</v>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="L20" s="5" t="n">
         <v>65</v>
       </c>
-      <c r="L20" s="14"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1288,34 +1166,37 @@
       <c r="B21" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15" t="n">
+      <c r="C21" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="13" t="n">
         <v>78</v>
       </c>
-      <c r="F21" s="15" t="n">
+      <c r="G21" s="13" t="n">
         <v>2297</v>
       </c>
-      <c r="G21" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="19" t="n">
+      <c r="H21" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" s="17" t="n">
         <v>50</v>
       </c>
-      <c r="I21" s="19" t="n">
-        <v>96</v>
-      </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" s="17" t="n">
+        <v>96</v>
+      </c>
+      <c r="K21" s="5" t="n">
         <v>8.1</v>
       </c>
-      <c r="K21" s="5" t="n">
+      <c r="L21" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="L21" s="14"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1324,34 +1205,37 @@
       <c r="B22" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="15" t="n">
+      <c r="C22" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="13" t="n">
         <v>75</v>
       </c>
-      <c r="F22" s="15" t="n">
+      <c r="G22" s="13" t="n">
         <v>2209</v>
       </c>
-      <c r="G22" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H22" s="19" t="n">
+      <c r="H22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" s="17" t="n">
         <v>50</v>
       </c>
-      <c r="I22" s="19" t="n">
-        <v>96</v>
-      </c>
-      <c r="J22" s="5" t="n">
+      <c r="J22" s="17" t="n">
+        <v>96</v>
+      </c>
+      <c r="K22" s="5" t="n">
         <v>8.1</v>
       </c>
-      <c r="K22" s="5" t="n">
+      <c r="L22" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="L22" s="14"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1360,34 +1244,37 @@
       <c r="B23" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="16" t="n">
+      <c r="C23" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="D23" s="16" t="n">
+      <c r="D23" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="E23" s="15" t="n">
+      <c r="E23" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13" t="n">
         <v>47</v>
       </c>
-      <c r="F23" s="15" t="n">
+      <c r="G23" s="13" t="n">
         <v>1384</v>
       </c>
-      <c r="G23" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H23" s="19" t="n">
-        <v>80</v>
-      </c>
-      <c r="I23" s="19" t="n">
+      <c r="H23" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" s="17" t="n">
+        <v>80</v>
+      </c>
+      <c r="J23" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="J23" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="K23" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5" t="n">
         <v>56</v>
       </c>
-      <c r="L23" s="14"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1396,34 +1283,37 @@
       <c r="B24" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C24" s="16" t="n">
+      <c r="C24" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="D24" s="16" t="n">
+      <c r="D24" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="E24" s="13" t="n">
+      <c r="E24" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11" t="n">
         <v>47</v>
       </c>
-      <c r="F24" s="13" t="n">
+      <c r="G24" s="11" t="n">
         <v>1384</v>
       </c>
-      <c r="G24" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H24" s="19" t="n">
-        <v>80</v>
-      </c>
-      <c r="I24" s="19" t="n">
+      <c r="H24" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I24" s="17" t="n">
+        <v>80</v>
+      </c>
+      <c r="J24" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="K24" s="5" t="n">
         <v>0.4</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="L24" s="5" t="n">
         <v>55.5</v>
       </c>
-      <c r="L24" s="14"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1432,34 +1322,37 @@
       <c r="B25" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D25" s="18" t="n">
+      <c r="D25" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="15" t="n">
+      <c r="E25" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13" t="n">
         <v>50</v>
       </c>
-      <c r="F25" s="15" t="n">
+      <c r="G25" s="13" t="n">
         <v>1473</v>
       </c>
-      <c r="G25" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H25" s="19" t="n">
-        <v>80</v>
-      </c>
-      <c r="I25" s="19" t="n">
+      <c r="H25" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I25" s="17" t="n">
+        <v>80</v>
+      </c>
+      <c r="J25" s="17" t="n">
         <v>95</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="K25" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="L25" s="5" t="n">
         <v>52.5</v>
       </c>
-      <c r="L25" s="14"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1468,37 +1361,38 @@
       <c r="B26" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C26" s="18" t="n">
+      <c r="C26" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="18" t="n">
+      <c r="D26" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E26" s="15" t="n">
+      <c r="E26" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="13" t="n">
         <v>47</v>
       </c>
-      <c r="F26" s="15" t="n">
+      <c r="G26" s="13" t="n">
         <v>1384</v>
       </c>
-      <c r="G26" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H26" s="19" t="n">
-        <v>80</v>
+      <c r="H26" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="I26" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="J26" s="5" t="n">
+        <v>80</v>
+      </c>
+      <c r="J26" s="15" t="n">
+        <v>96</v>
+      </c>
+      <c r="K26" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="K26" s="5" t="n">
+      <c r="L26" s="5" t="n">
         <v>49</v>
       </c>
-      <c r="L26" s="14"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="M26" s="12"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>